<commit_message>
Added new Features to Inventory
</commit_message>
<xml_diff>
--- a/inventory.xlsx
+++ b/inventory.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\github\py\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B0B9894-B86D-4B96-B10D-5AFFBB41F32F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01C4FC7C-E4C0-4E01-8ABB-A55CE35229C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Inventory" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="181029"/>
 </workbook>
 </file>
 
@@ -65,10 +65,17 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -94,8 +101,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -398,10 +406,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="B40" sqref="B40:D40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -433,6 +441,10 @@
       <c r="C2">
         <v>70</v>
       </c>
+      <c r="D2">
+        <f>PRODUCT(B2:C2)</f>
+        <v>350</v>
+      </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
@@ -444,6 +456,10 @@
       <c r="C3">
         <v>90</v>
       </c>
+      <c r="D3">
+        <f t="shared" ref="D3:D10" si="0">PRODUCT(B3:C3)</f>
+        <v>90</v>
+      </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
@@ -455,6 +471,10 @@
       <c r="C4">
         <v>50</v>
       </c>
+      <c r="D4">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
@@ -466,6 +486,10 @@
       <c r="C5">
         <v>60</v>
       </c>
+      <c r="D5">
+        <f t="shared" si="0"/>
+        <v>300</v>
+      </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
@@ -477,6 +501,10 @@
       <c r="C6">
         <v>85</v>
       </c>
+      <c r="D6">
+        <f t="shared" si="0"/>
+        <v>425</v>
+      </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
@@ -488,6 +516,10 @@
       <c r="C7">
         <v>100</v>
       </c>
+      <c r="D7">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
@@ -499,6 +531,10 @@
       <c r="C8">
         <v>65</v>
       </c>
+      <c r="D8">
+        <f t="shared" si="0"/>
+        <v>325</v>
+      </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
@@ -510,6 +546,10 @@
       <c r="C9">
         <v>75</v>
       </c>
+      <c r="D9">
+        <f t="shared" si="0"/>
+        <v>375</v>
+      </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
@@ -520,6 +560,24 @@
       </c>
       <c r="C10">
         <v>75</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="0"/>
+        <v>375</v>
+      </c>
+    </row>
+    <row r="40" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B40">
+        <f>SUM(B2:B10)</f>
+        <v>34</v>
+      </c>
+      <c r="C40">
+        <f>SUM(C2:C10)</f>
+        <v>670</v>
+      </c>
+      <c r="D40" s="1">
+        <f>SUM(D2:D10)</f>
+        <v>2440</v>
       </c>
     </row>
   </sheetData>

</xml_diff>